<commit_message>
Finished with genre adding / removing
</commit_message>
<xml_diff>
--- a/Book.xlsx
+++ b/Book.xlsx
@@ -727,10 +727,10 @@
       </c>
     </row>
     <row r="3" ht="13.5" customHeight="1" s="3">
-      <c r="A3" t="n">
+      <c r="A3" s="2" t="n">
         <v>915160401</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="n">
@@ -746,7 +746,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="2" t="n">
         <v>0</v>
@@ -767,7 +767,7 @@
         <v>0</v>
       </c>
       <c r="N3" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O3" s="2" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Addition to last commit: changed "Support" sticker
</commit_message>
<xml_diff>
--- a/Book.xlsx
+++ b/Book.xlsx
@@ -743,10 +743,10 @@
         <v>0</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" s="2" t="n">
         <v>0</v>

</xml_diff>